<commit_message>
Housing Price Prediction Kaggle Competition
</commit_message>
<xml_diff>
--- a/Titanic Survival Prediction/output_neural.xlsx
+++ b/Titanic Survival Prediction/output_neural.xlsx
@@ -428,7 +428,7 @@
         <v>896</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -540,7 +540,7 @@
         <v>910</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -588,7 +588,7 @@
         <v>916</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -604,7 +604,7 @@
         <v>918</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -780,7 +780,7 @@
         <v>940</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -812,7 +812,7 @@
         <v>944</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -820,7 +820,7 @@
         <v>945</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -868,7 +868,7 @@
         <v>951</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -924,7 +924,7 @@
         <v>958</v>
       </c>
       <c r="B68">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -948,7 +948,7 @@
         <v>961</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -988,7 +988,7 @@
         <v>966</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1132,7 +1132,7 @@
         <v>984</v>
       </c>
       <c r="B94">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1164,7 +1164,7 @@
         <v>988</v>
       </c>
       <c r="B98">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1196,7 +1196,7 @@
         <v>992</v>
       </c>
       <c r="B102">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1292,7 +1292,7 @@
         <v>1004</v>
       </c>
       <c r="B114">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1308,7 +1308,7 @@
         <v>1006</v>
       </c>
       <c r="B116">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1372,7 +1372,7 @@
         <v>1014</v>
       </c>
       <c r="B124">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1524,7 +1524,7 @@
         <v>1033</v>
       </c>
       <c r="B143">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -1596,7 +1596,7 @@
         <v>1042</v>
       </c>
       <c r="B152">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -1620,7 +1620,7 @@
         <v>1045</v>
       </c>
       <c r="B155">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -1644,7 +1644,7 @@
         <v>1048</v>
       </c>
       <c r="B158">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -1668,7 +1668,7 @@
         <v>1051</v>
       </c>
       <c r="B161">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -1740,7 +1740,7 @@
         <v>1060</v>
       </c>
       <c r="B170">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -1828,7 +1828,7 @@
         <v>1071</v>
       </c>
       <c r="B181">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -1868,7 +1868,7 @@
         <v>1076</v>
       </c>
       <c r="B186">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -2060,7 +2060,7 @@
         <v>1100</v>
       </c>
       <c r="B210">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -2108,7 +2108,7 @@
         <v>1106</v>
       </c>
       <c r="B216">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -2140,7 +2140,7 @@
         <v>1110</v>
       </c>
       <c r="B220">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -2156,7 +2156,7 @@
         <v>1112</v>
       </c>
       <c r="B222">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -2188,7 +2188,7 @@
         <v>1116</v>
       </c>
       <c r="B226">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="227" spans="1:2">
@@ -2300,7 +2300,7 @@
         <v>1130</v>
       </c>
       <c r="B240">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -2308,7 +2308,7 @@
         <v>1131</v>
       </c>
       <c r="B241">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="242" spans="1:2">
@@ -2316,7 +2316,7 @@
         <v>1132</v>
       </c>
       <c r="B242">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="243" spans="1:2">
@@ -2500,7 +2500,7 @@
         <v>1155</v>
       </c>
       <c r="B265">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="266" spans="1:2">
@@ -2572,7 +2572,7 @@
         <v>1164</v>
       </c>
       <c r="B274">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="275" spans="1:2">
@@ -2908,7 +2908,7 @@
         <v>1206</v>
       </c>
       <c r="B316">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="317" spans="1:2">
@@ -2988,7 +2988,7 @@
         <v>1216</v>
       </c>
       <c r="B326">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="327" spans="1:2">
@@ -3140,7 +3140,7 @@
         <v>1235</v>
       </c>
       <c r="B345">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="346" spans="1:2">
@@ -3172,7 +3172,7 @@
         <v>1239</v>
       </c>
       <c r="B349">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="350" spans="1:2">
@@ -3196,7 +3196,7 @@
         <v>1242</v>
       </c>
       <c r="B352">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="353" spans="1:2">
@@ -3308,7 +3308,7 @@
         <v>1256</v>
       </c>
       <c r="B366">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="367" spans="1:2">
@@ -3340,7 +3340,7 @@
         <v>1260</v>
       </c>
       <c r="B370">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="371" spans="1:2">
@@ -3364,7 +3364,7 @@
         <v>1263</v>
       </c>
       <c r="B373">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="374" spans="1:2">
@@ -3396,7 +3396,7 @@
         <v>1267</v>
       </c>
       <c r="B377">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="378" spans="1:2">
@@ -3572,7 +3572,7 @@
         <v>1289</v>
       </c>
       <c r="B399">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="400" spans="1:2">
@@ -3596,7 +3596,7 @@
         <v>1292</v>
       </c>
       <c r="B402">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="403" spans="1:2">
@@ -3612,7 +3612,7 @@
         <v>1294</v>
       </c>
       <c r="B404">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="405" spans="1:2">
@@ -3668,7 +3668,7 @@
         <v>1301</v>
       </c>
       <c r="B411">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="412" spans="1:2">
@@ -3684,7 +3684,7 @@
         <v>1303</v>
       </c>
       <c r="B413">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="414" spans="1:2">
@@ -3708,7 +3708,7 @@
         <v>1306</v>
       </c>
       <c r="B416">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="417" spans="1:2">

</xml_diff>